<commit_message>
Add validation checks for Excel cell formatting and formula errors
</commit_message>
<xml_diff>
--- a/rspec/fixtures/test.xlsx
+++ b/rspec/fixtures/test.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -191,9 +194,6 @@
     <t>title2</t>
   </si>
   <si>
-    <t>#VALUE?</t>
-  </si>
-  <si>
     <t>bad type</t>
   </si>
   <si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>cats</t>
+  </si>
+  <si>
+    <t>2/2/1902</t>
   </si>
 </sst>
 </file>
@@ -257,9 +260,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -275,6 +279,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet2"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -543,7 +560,7 @@
   <dimension ref="A1:AQ5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AQ5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,43 +750,51 @@
         <v>54</v>
       </c>
       <c r="D4" t="e">
+        <f>VLOOKUP(A4,B:B,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="E4" t="e">
+        <f>[1]Sheet2!A1</f>
         <v>#REF!</v>
+      </c>
+      <c r="G4">
+        <f>F4</f>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4" t="e">
+        <f>a+b</f>
         <v>#NAME?</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="e">
+        <f>K4+5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K4" t="s">
         <v>55</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>56</v>
       </c>
-      <c r="L4" t="s">
+      <c r="O4" t="s">
         <v>57</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>58</v>
       </c>
-      <c r="P4" t="s">
+      <c r="R4" t="s">
         <v>59</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>60</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>61</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>62</v>
-      </c>
-      <c r="U4" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.25">
@@ -783,13 +808,13 @@
         <v>43</v>
       </c>
       <c r="D5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" t="s">
         <v>64</v>
       </c>
-      <c r="H5" t="s">
-        <v>65</v>
-      </c>
       <c r="N5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q5" s="1">
         <v>1</v>
@@ -799,6 +824,9 @@
       </c>
       <c r="S5" t="s">
         <v>50</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="Y5">
         <v>1905</v>
@@ -809,5 +837,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>